<commit_message>
update template, concatenate reissue dates
</commit_message>
<xml_diff>
--- a/backend/src/static/templates/reports/Dairy_Client_Details_Template.xlsx
+++ b/backend/src/static/templates/reports/Dairy_Client_Details_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\backend\src\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37768DC4-D820-451A-A32B-9E6E893A1D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6895179-3A23-4D53-AF93-1A2E6148E29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="38700" windowHeight="15345" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="29370" windowHeight="15345" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>IH</t>
   </si>
@@ -431,16 +431,10 @@
     <t>{ d.Client[i+1]:ifNEM():show(License Re-Issued:) }</t>
   </si>
   <si>
-    <t>{d.Client[i].ReissueDates[i].date}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].ReissueDates[i+1].date}</t>
-  </si>
-  <si>
-    <t>{d.Client[i+1].ReissueDates[i].date}</t>
-  </si>
-  <si>
-    <t>{d.Client[i+1].ReissueDates[i+1].date}</t>
+    <t>{d.Client[i+1].ReissueDates</t>
+  </si>
+  <si>
+    <t>{d.Client[i].ReissueDates}</t>
   </si>
 </sst>
 </file>
@@ -889,7 +883,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,20 +953,18 @@
         <v>130</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="26" t="s">
-        <v>133</v>
-      </c>
+      <c r="F6" s="26"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
@@ -1289,7 +1281,7 @@
         <v>131</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G31" s="5"/>
     </row>
@@ -1299,9 +1291,7 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="26" t="s">
-        <v>135</v>
-      </c>
+      <c r="F32" s="26"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -1582,21 +1572,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -1819,7 +1794,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2AF8CD6-3E38-48DB-89EE-EAD5D47F2F99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137977AE-5CF3-42F0-AD7C-49AF06AF507F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1836,29 +1845,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2AF8CD6-3E38-48DB-89EE-EAD5D47F2F99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>